<commit_message>
sugeno 3-class result added for version 1 & 3
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Team-8-CDFSI\T8_CDSFI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBA70F8-82BC-4AEF-9C6A-6D3A9437F666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A36CBFA-96DA-4D19-9D5E-5AB00F99C5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -158,9 +158,6 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -170,6 +167,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -454,751 +454,787 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B61" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView tabSelected="1" topLeftCell="B58" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="L77" sqref="L77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="27" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="27" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="34.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>0.57079999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>0.875</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>0.88</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>0.88</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>0.88</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>0.94220000000000004</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>0.9415</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>0.89670000000000005</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>0.9</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>0.9</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>0.9</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>0.94030000000000002</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <v>0.93579999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>0.90210000000000001</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>0.9</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>0.9</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>0.9</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>0.93979999999999997</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>0.93799999999999994</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>0.80969999999999998</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>0.81</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>0.81</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>0.81</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>0.89710000000000001</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <v>0.90780000000000005</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>0.81520000000000004</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>0.81</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>0.81</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>0.82</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <v>0.81179999999999997</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="1">
         <v>0.87849999999999995</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>0.88039999999999996</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>0.88</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>0.88</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>0.88</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <v>0.9425</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="1">
         <v>0.94750000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>0.73360000000000003</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>0.73</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>0.73</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>0.73</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <v>0.75509999999999999</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="1">
         <v>0.76019999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>0.875</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>0.87</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>0.87</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>0.88</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="1">
         <v>0.91</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="1">
         <v>0.88260000000000005</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="C20" s="1">
+        <v>0.90759999999999996</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.90469999999999995</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.93700000000000006</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="34.5" x14ac:dyDescent="0.45">
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G38" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H38" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="1">
         <v>0.48420000000000002</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="1">
         <v>0.83599999999999997</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="1">
         <v>0.84</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="1">
         <v>0.84</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="1">
         <v>0.84</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41" s="1">
         <v>0.89390000000000003</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41" s="1">
         <v>0.88329999999999997</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="1">
         <v>0.86880000000000002</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="1">
         <v>0.87</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="1">
         <v>0.87</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42" s="1">
         <v>0.87</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="1">
         <v>0.88849999999999996</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="1">
         <v>0.87290000000000001</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="1">
         <v>0.88519999999999999</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="1">
         <v>0.88</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43" s="1">
         <v>0.89</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F43" s="1">
         <v>0.89</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G43" s="1">
         <v>0.88959999999999995</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="1">
         <v>0.88419999999999999</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="1">
         <v>0.8196</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="1">
         <v>0.82</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44" s="1">
         <v>0.82</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F44" s="1">
         <v>0.82</v>
       </c>
-      <c r="G44" s="2">
+      <c r="G44" s="1">
         <v>0.89059999999999995</v>
       </c>
-      <c r="H44" s="2">
+      <c r="H44" s="1">
         <v>0.87490000000000001</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="1">
         <v>0.8196</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="1">
         <v>0.82</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45" s="1">
         <v>0.82</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F45" s="1">
         <v>0.82</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G45" s="1">
         <v>0.81699999999999995</v>
       </c>
-      <c r="H45" s="2">
+      <c r="H45" s="1">
         <v>0.87690000000000001</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="1">
         <v>0.83599999999999997</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="1">
         <v>0.83</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46" s="1">
         <v>0.84</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F46" s="1">
         <v>0.84</v>
       </c>
-      <c r="G46" s="2">
+      <c r="G46" s="1">
         <v>0.91500000000000004</v>
       </c>
-      <c r="H46" s="2">
+      <c r="H46" s="1">
         <v>0.91620000000000001</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="1">
         <v>0.65569999999999995</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="1">
         <v>0.65</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E47" s="1">
         <v>0.66</v>
       </c>
-      <c r="F47" s="2">
+      <c r="F47" s="1">
         <v>0.66</v>
       </c>
-      <c r="G47" s="2">
+      <c r="G47" s="1">
         <v>0.6996</v>
       </c>
-      <c r="H47" s="2">
+      <c r="H47" s="1">
         <v>0.76419999999999999</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="1">
         <v>0.86880000000000002</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48" s="1">
         <v>0.87</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E48" s="1">
         <v>0.87</v>
       </c>
-      <c r="F48" s="2">
+      <c r="F48" s="1">
         <v>0.87</v>
       </c>
-      <c r="G48" s="2">
+      <c r="G48" s="1">
         <v>0.87009999999999998</v>
       </c>
-      <c r="H48" s="2">
+      <c r="H48" s="1">
         <v>0.8337</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="57" spans="2:8" ht="34.5" x14ac:dyDescent="0.45">
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="2:8" ht="42.75" x14ac:dyDescent="0.8">
-      <c r="B60" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
+      <c r="B60" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="F62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G62" s="3" t="s">
+      <c r="G62" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H62" s="3" t="s">
+      <c r="H62" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="1">
         <v>0.50670000000000004</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65" s="1">
         <v>0.83899999999999997</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D65" s="1">
         <v>0.84</v>
       </c>
-      <c r="E65" s="2">
+      <c r="E65" s="1">
         <v>0.84</v>
       </c>
-      <c r="F65" s="2">
+      <c r="F65" s="1">
         <v>0.84</v>
       </c>
-      <c r="G65" s="2">
+      <c r="G65" s="1">
         <v>0.92159999999999997</v>
       </c>
-      <c r="H65" s="2">
+      <c r="H65" s="1">
         <v>0.91159999999999997</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66" s="1">
         <v>0.83899999999999997</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D66" s="1">
         <v>0.84</v>
       </c>
-      <c r="E66" s="2">
+      <c r="E66" s="1">
         <v>0.85</v>
       </c>
-      <c r="F66" s="2">
+      <c r="F66" s="1">
         <v>0.84</v>
       </c>
-      <c r="G66" s="2">
+      <c r="G66" s="1">
         <v>0.92190000000000005</v>
       </c>
-      <c r="H66" s="2">
+      <c r="H66" s="1">
         <v>0.90369999999999995</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67" s="1">
         <v>0.82920000000000005</v>
       </c>
-      <c r="D67" s="2">
+      <c r="D67" s="1">
         <v>0.83</v>
       </c>
-      <c r="E67" s="2">
+      <c r="E67" s="1">
         <v>0.84</v>
       </c>
-      <c r="F67" s="2">
+      <c r="F67" s="1">
         <v>0.83</v>
       </c>
-      <c r="G67" s="2">
+      <c r="G67" s="1">
         <v>0.91139999999999999</v>
       </c>
-      <c r="H67" s="2">
+      <c r="H67" s="1">
         <v>0.90280000000000005</v>
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68" s="1">
         <v>0.82430000000000003</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D68" s="1">
         <v>0.82</v>
       </c>
-      <c r="E68" s="2">
+      <c r="E68" s="1">
         <v>0.83</v>
       </c>
-      <c r="F68" s="2">
+      <c r="F68" s="1">
         <v>0.82</v>
       </c>
-      <c r="G68" s="2">
+      <c r="G68" s="1">
         <v>0.89270000000000005</v>
       </c>
-      <c r="H68" s="2">
+      <c r="H68" s="1">
         <v>0.86919999999999997</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C69" s="2">
-        <v>1</v>
-      </c>
-      <c r="D69" s="2">
-        <v>1</v>
-      </c>
-      <c r="E69" s="2">
-        <v>1</v>
-      </c>
-      <c r="F69" s="2">
-        <v>1</v>
-      </c>
-      <c r="G69" s="2">
-        <v>1</v>
-      </c>
-      <c r="H69" s="2">
+      <c r="C69" s="1">
+        <v>1</v>
+      </c>
+      <c r="D69" s="1">
+        <v>1</v>
+      </c>
+      <c r="E69" s="1">
+        <v>1</v>
+      </c>
+      <c r="F69" s="1">
+        <v>1</v>
+      </c>
+      <c r="G69" s="1">
+        <v>1</v>
+      </c>
+      <c r="H69" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="2">
-        <v>1</v>
-      </c>
-      <c r="D70" s="2">
-        <v>1</v>
-      </c>
-      <c r="E70" s="2">
-        <v>1</v>
-      </c>
-      <c r="F70" s="2">
-        <v>1</v>
-      </c>
-      <c r="G70" s="2">
-        <v>1</v>
-      </c>
-      <c r="H70" s="2">
+      <c r="C70" s="1">
+        <v>1</v>
+      </c>
+      <c r="D70" s="1">
+        <v>1</v>
+      </c>
+      <c r="E70" s="1">
+        <v>1</v>
+      </c>
+      <c r="F70" s="1">
+        <v>1</v>
+      </c>
+      <c r="G70" s="1">
+        <v>1</v>
+      </c>
+      <c r="H70" s="1">
         <v>0.99990000000000001</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71" s="1">
         <v>0.72189999999999999</v>
       </c>
-      <c r="D71" s="2">
+      <c r="D71" s="1">
         <v>0.72</v>
       </c>
-      <c r="E71" s="2">
+      <c r="E71" s="1">
         <v>0.72</v>
       </c>
-      <c r="F71" s="2">
+      <c r="F71" s="1">
         <v>0.72</v>
       </c>
-      <c r="G71" s="2">
+      <c r="G71" s="1">
         <v>0.86819999999999997</v>
       </c>
-      <c r="H71" s="2">
+      <c r="H71" s="1">
         <v>0.89449999999999996</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72" s="1">
         <v>0.85360000000000003</v>
       </c>
-      <c r="D72" s="2">
+      <c r="D72" s="1">
         <v>0.85</v>
       </c>
-      <c r="E72" s="2">
+      <c r="E72" s="1">
         <v>0.86</v>
       </c>
-      <c r="F72" s="2">
+      <c r="F72" s="1">
         <v>0.85</v>
       </c>
-      <c r="G72" s="2">
+      <c r="G72" s="1">
         <v>0.91600000000000004</v>
       </c>
-      <c r="H72" s="2">
+      <c r="H72" s="1">
         <v>0.91679999999999995</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="C75" s="1">
+        <v>0.86819999999999997</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="E75" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="F75" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="G75" s="1">
+        <v>0.8659</v>
+      </c>
+      <c r="H75" s="1">
+        <v>0.89790000000000003</v>
+      </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="2" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sfi emsemnle experiment done
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Team-8-CDFSI\T8_CDSFI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Md Obaidul Isl\Desktop\My Research\T8_CDSFI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A36CBFA-96DA-4D19-9D5E-5AB00F99C5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1811C46D-239A-44AF-AC53-6C8345CEE183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="28">
   <si>
     <t>TRAIN SET SIZE</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t>ACCURACY</t>
+  </si>
+  <si>
+    <t>Majority Voting</t>
+  </si>
+  <si>
+    <t>Stacking</t>
+  </si>
+  <si>
+    <t>Bagging</t>
+  </si>
+  <si>
+    <t>Weighted Average</t>
   </si>
 </sst>
 </file>
@@ -156,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -171,6 +183,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -452,25 +467,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H77"/>
+  <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B58" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="L77" sqref="L77"/>
+    <sheetView tabSelected="1" topLeftCell="B82" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
     <col min="2" max="2" width="27" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="3" width="11.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="34.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
@@ -478,17 +493,23 @@
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="2">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
@@ -508,7 +529,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
@@ -516,7 +537,7 @@
         <v>0.57079999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -539,7 +560,7 @@
         <v>0.9415</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
@@ -562,7 +583,7 @@
         <v>0.93579999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
@@ -585,7 +606,7 @@
         <v>0.93799999999999994</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
@@ -608,7 +629,7 @@
         <v>0.90780000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
@@ -631,7 +652,7 @@
         <v>0.87849999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
@@ -654,7 +675,7 @@
         <v>0.94750000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
@@ -677,7 +698,7 @@
         <v>0.76019999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
@@ -700,12 +721,12 @@
         <v>0.88260000000000005</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="1">
-        <v>0.90759999999999996</v>
+        <v>0.90760869565217395</v>
       </c>
       <c r="D20" s="1">
         <v>0.91</v>
@@ -723,32 +744,94 @@
         <v>0.93700000000000006</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <v>0.91304347826086896</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.91319942611190796</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.94533887468030697</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" ht="34.5" x14ac:dyDescent="0.45">
+      <c r="C22" s="2">
+        <v>0.90760869565217395</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.90351506456241004</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0.93549071396132599</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C38" s="2" t="s">
         <v>23</v>
       </c>
@@ -768,7 +851,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
@@ -776,7 +859,7 @@
         <v>0.48420000000000002</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
         <v>7</v>
       </c>
@@ -799,7 +882,7 @@
         <v>0.88329999999999997</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
         <v>2</v>
       </c>
@@ -822,7 +905,7 @@
         <v>0.87290000000000001</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
         <v>21</v>
       </c>
@@ -845,7 +928,7 @@
         <v>0.88419999999999999</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B44" s="3" t="s">
         <v>22</v>
       </c>
@@ -868,7 +951,7 @@
         <v>0.87490000000000001</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
         <v>4</v>
       </c>
@@ -891,7 +974,7 @@
         <v>0.87690000000000001</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
         <v>5</v>
       </c>
@@ -914,7 +997,7 @@
         <v>0.91620000000000001</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
         <v>8</v>
       </c>
@@ -937,7 +1020,7 @@
         <v>0.76419999999999999</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
         <v>3</v>
       </c>
@@ -960,282 +1043,417 @@
         <v>0.8337</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C50" s="2">
+        <v>0.90163934426229497</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="E50" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="G50" s="2">
+        <v>0.89556277056277001</v>
+      </c>
+      <c r="H50" s="2">
+        <v>0.92547763859239196</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B51" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <v>0.90163934426229497</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E51" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="G51" s="2">
+        <v>0.89826839826839799</v>
+      </c>
+      <c r="H51" s="2">
+        <v>0.92894755517706296</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B52" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="57" spans="2:8" ht="34.5" x14ac:dyDescent="0.45">
-      <c r="B57" s="4" t="s">
+      <c r="C52" s="2">
+        <v>0.88524590163934402</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="E52" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="G52" s="2">
+        <v>0.88041125541125498</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0.91664596787547603</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B53" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B54" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B55" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B56" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
+      <c r="B78" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="2" t="s">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B80" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="2:8" ht="42.75" x14ac:dyDescent="0.8">
-      <c r="B60" s="2" t="s">
+      <c r="C80" s="2">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" ht="43.8" x14ac:dyDescent="1.05">
+      <c r="B81" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C62" s="2" t="s">
+      <c r="C81" s="7">
+        <v>205</v>
+      </c>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C83" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="E83" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F62" s="2" t="s">
+      <c r="F83" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="G83" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H62" s="2" t="s">
+      <c r="H83" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="2" t="s">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B85" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C85" s="1">
         <v>0.50670000000000004</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B65" s="2" t="s">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B86" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C86" s="1">
         <v>0.83899999999999997</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D86" s="1">
         <v>0.84</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E86" s="1">
         <v>0.84</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F86" s="1">
         <v>0.84</v>
       </c>
-      <c r="G65" s="1">
+      <c r="G86" s="1">
         <v>0.92159999999999997</v>
       </c>
-      <c r="H65" s="1">
+      <c r="H86" s="1">
         <v>0.91159999999999997</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="2" t="s">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B87" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C87" s="1">
         <v>0.83899999999999997</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D87" s="1">
         <v>0.84</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E87" s="1">
         <v>0.85</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F87" s="1">
         <v>0.84</v>
       </c>
-      <c r="G66" s="1">
+      <c r="G87" s="1">
         <v>0.92190000000000005</v>
       </c>
-      <c r="H66" s="1">
+      <c r="H87" s="1">
         <v>0.90369999999999995</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="2" t="s">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B88" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C88" s="1">
         <v>0.82920000000000005</v>
       </c>
-      <c r="D67" s="1">
+      <c r="D88" s="1">
         <v>0.83</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E88" s="1">
         <v>0.84</v>
       </c>
-      <c r="F67" s="1">
+      <c r="F88" s="1">
         <v>0.83</v>
       </c>
-      <c r="G67" s="1">
+      <c r="G88" s="1">
         <v>0.91139999999999999</v>
       </c>
-      <c r="H67" s="1">
+      <c r="H88" s="1">
         <v>0.90280000000000005</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="3" t="s">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B89" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="1">
+      <c r="C89" s="1">
         <v>0.82430000000000003</v>
       </c>
-      <c r="D68" s="1">
+      <c r="D89" s="1">
         <v>0.82</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E89" s="1">
         <v>0.83</v>
       </c>
-      <c r="F68" s="1">
+      <c r="F89" s="1">
         <v>0.82</v>
       </c>
-      <c r="G68" s="1">
+      <c r="G89" s="1">
         <v>0.89270000000000005</v>
       </c>
-      <c r="H68" s="1">
+      <c r="H89" s="1">
         <v>0.86919999999999997</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="2" t="s">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B90" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C90" s="1">
         <v>1</v>
       </c>
-      <c r="D69" s="1">
+      <c r="D90" s="1">
         <v>1</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E90" s="1">
         <v>1</v>
       </c>
-      <c r="F69" s="1">
+      <c r="F90" s="1">
         <v>1</v>
       </c>
-      <c r="G69" s="1">
+      <c r="G90" s="1">
         <v>1</v>
       </c>
-      <c r="H69" s="1">
+      <c r="H90" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="2" t="s">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B91" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="1">
+      <c r="C91" s="1">
         <v>1</v>
       </c>
-      <c r="D70" s="1">
+      <c r="D91" s="1">
         <v>1</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E91" s="1">
         <v>1</v>
       </c>
-      <c r="F70" s="1">
+      <c r="F91" s="1">
         <v>1</v>
       </c>
-      <c r="G70" s="1">
+      <c r="G91" s="1">
         <v>1</v>
       </c>
-      <c r="H70" s="1">
+      <c r="H91" s="1">
         <v>0.99990000000000001</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B71" s="2" t="s">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B92" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C71" s="1">
+      <c r="C92" s="1">
         <v>0.72189999999999999</v>
       </c>
-      <c r="D71" s="1">
+      <c r="D92" s="1">
         <v>0.72</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E92" s="1">
         <v>0.72</v>
       </c>
-      <c r="F71" s="1">
+      <c r="F92" s="1">
         <v>0.72</v>
       </c>
-      <c r="G71" s="1">
+      <c r="G92" s="1">
         <v>0.86819999999999997</v>
       </c>
-      <c r="H71" s="1">
+      <c r="H92" s="1">
         <v>0.89449999999999996</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B72" s="2" t="s">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B93" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C72" s="1">
+      <c r="C93" s="1">
         <v>0.85360000000000003</v>
       </c>
-      <c r="D72" s="1">
+      <c r="D93" s="1">
         <v>0.85</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E93" s="1">
         <v>0.86</v>
       </c>
-      <c r="F72" s="1">
+      <c r="F93" s="1">
         <v>0.85</v>
       </c>
-      <c r="G72" s="1">
+      <c r="G93" s="1">
         <v>0.91600000000000004</v>
       </c>
-      <c r="H72" s="1">
+      <c r="H93" s="1">
         <v>0.91679999999999995</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="2" t="s">
+    <row r="96" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B96" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C75" s="1">
-        <v>0.86819999999999997</v>
-      </c>
-      <c r="D75" s="1">
+      <c r="C96" s="1">
+        <v>0.86829268292682904</v>
+      </c>
+      <c r="D96" s="1">
         <v>0.87</v>
       </c>
-      <c r="E75" s="1">
+      <c r="E96" s="1">
         <v>0.88</v>
       </c>
-      <c r="F75" s="1">
+      <c r="F96" s="1">
         <v>0.87</v>
       </c>
-      <c r="G75" s="1">
+      <c r="G96" s="1">
         <v>0.8659</v>
       </c>
-      <c r="H75" s="1">
+      <c r="H96" s="1">
         <v>0.89790000000000003</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="2" t="s">
+    <row r="97" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B97" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B77" s="2" t="s">
+      <c r="C97" s="2">
+        <v>0.87317073170731696</v>
+      </c>
+      <c r="D97" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="E97" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="F97" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G97" s="2">
+        <v>0.87095238095238103</v>
+      </c>
+      <c r="H97" s="2">
+        <v>0.90127758420441295</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B98" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="C98" s="2">
+        <v>0.85365853658536495</v>
+      </c>
+      <c r="D98" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="E98" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="F98" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="G98" s="2">
+        <v>0.85238095238095202</v>
+      </c>
+      <c r="H98" s="2">
+        <v>0.889814674544261</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B99" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B100" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B101" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B102" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>